<commit_message>
updates done 2:40pm 03-02-2026
</commit_message>
<xml_diff>
--- a/Excel Output/Hotels Sort Verification Details.xlsx
+++ b/Excel Output/Hotels Sort Verification Details.xlsx
@@ -152,8 +152,8 @@
 2 bedrooms
 2 beds
 Free Cancellation
-Earn ₹ 961.74 in Trip Coins
-Last booked 5 hrs ago
+Earn ₹ 962.30 in Trip Coins
+Last booked 6 hrs ago
 Limited Time Offer
 15% off
 ₹ 19,625
@@ -286,7 +286,7 @@
 2 beds
 Free Cancellation
 Breakfast included
-Earn ₹ 1,322.62 in Trip Coins
+Earn ₹ 1,323.05 in Trip Coins
 Only 5 left at this price
 Special Discount
 8% off
@@ -327,7 +327,7 @@
 Entire apartment 95㎡
 2 bedrooms
 3 beds
-Earn ₹ 546.73 in Trip Coins
+Earn ₹ 546.53 in Trip Coins
 Only 3 left at this price
 Special Discount
 11% off
@@ -514,7 +514,7 @@
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s" s="0">
         <v>9</v>
@@ -525,7 +525,7 @@
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s" s="0">
         <v>11</v>

</xml_diff>

<commit_message>
Extent reports added to jenkins and Updated testClasses
</commit_message>
<xml_diff>
--- a/Excel Output/Hotels Sort Verification Details.xlsx
+++ b/Excel Output/Hotels Sort Verification Details.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="26">
   <si>
     <t>After Searched</t>
   </si>
@@ -34,10 +34,10 @@
 Breakfast included
 Only 1 left at this price
 Special Discount
-12% off
-₹ 6,189
-₹ 5,324
-Total price: ₹ 31,457
+10% off
+₹ 6,163
+₹ 5,489
+Total price: ₹ 32,440
 1 room × 5 nights incl. taxes &amp; fees
 Check Availability
 Sign in for member prices</t>
@@ -45,7 +45,7 @@
   <si>
     <t>Woodmere Serviced Apartment
 8.6/10
-Very good70 reviews
+Very good68 reviews
 Near Yaya CentreShow on Map
 Standard Two-Bedroom Apartment
 x4
@@ -68,7 +68,6 @@
 Family Room
 x4
 Free Cancellation
-Last booked 21 hrs ago
 ₹ 19,986
 Total price: ₹ 127,909
 1 room × 5 nights incl. taxes &amp; fees
@@ -114,7 +113,6 @@
 x4
 Free Cancellation
 Breakfast included
-Last booked 18 hrs ago
 ₹ 203,399
 Total price: ₹ 1,284,055
 1 room × 5 nights incl. taxes &amp; fees
@@ -150,7 +148,7 @@
 2 beds
 Free Cancellation
 Earn ₹ 962.26 in Trip Coins
-Last booked 8 hrs ago
+Last booked 14 hrs ago
 Limited Time Offer
 15% off
 ₹ 19,632
@@ -191,27 +189,58 @@
 Entire unit 108㎡
 2 bedrooms
 2 beds
-Last booked 5 hrs ago
+Last booked 3 hrs ago
 ₹ 23,235
 Total price: ₹ 145,219
 1 room × 5 nights incl. taxes &amp; fees
 Check Availability</t>
   </si>
   <si>
-    <t>Arcadia Hotel
-Renovated in 2025
-8.8/10
-Very good13 reviews
-Near Yaya CentreShow on Map
-Two-Bedroom Suite
-x4
-Entire unit 110㎡
+    <t>Kester International Apartment Hotel
+Opened in 2025
+9.8/10
+Outstanding28 reviews
+"Great service"
+"Great rooms"
+Near Yaya CentreShow on Map
+Boutique 2-bedroom And 1-living Room Suite
+x4
+Entire apartment 95㎡
+2 bedrooms
+3 beds
+Earn ₹ 547.03 in Trip Coins
+Only 3 left at this price
+Special Discount
+11% off
+₹ 7,141
+₹ 6,284
+Total price: ₹ 36,444
+1 room × 5 nights incl. taxes &amp; fees
+Check Availability
+Sign in for member prices</t>
+  </si>
+  <si>
+    <t>Lux Suites Riara One Residency Angama
+Opened in 2025
+9.9/10
+Outstanding17 reviews
+"Clean and tidy"
+"Great location"
+Near Yaya CentreShow on Map
+Family Room
+x4
+Entire apartment 98㎡
 2 bedrooms
 2 beds
 Free Cancellation
+Breakfast included
+Earn ₹ 1,323.34 in Trip Coins
 Only 5 left at this price
-₹ 7,704
-Total price: ₹ 44,682
+Special Discount
+8% off
+₹ 16,398
+₹ 14,946
+Total price: ₹ 88,178
 1 room × 5 nights incl. taxes &amp; fees
 Check Availability
 Sign in for member prices</t>
@@ -252,7 +281,6 @@
 Family Room
 x4
 Free Cancellation
-Last booked 21 hrs ago
 ₹ 19,986
 Total price: ₹ 127,909
 1 room × 5 nights incl. taxes &amp; fees
@@ -272,27 +300,20 @@
 Check Availability</t>
   </si>
   <si>
-    <t>Lux Suites Riara One Residency Angama
-Opened in 2025
-9.9/10
-Outstanding17 reviews
-"Clean and tidy"
-"Great location"
-Near Yaya CentreShow on Map
-Family Room
-x4
-Entire apartment 98㎡
+    <t>Arcadia Hotel
+Renovated in 2025
+8.8/10
+Very good13 reviews
+Near Yaya CentreShow on Map
+Two-Bedroom Suite
+x4
+Entire unit 110㎡
 2 bedrooms
 2 beds
 Free Cancellation
-Breakfast included
-Earn ₹ 1,323.34 in Trip Coins
 Only 5 left at this price
-Special Discount
-8% off
-₹ 16,398
-₹ 14,946
-Total price: ₹ 88,178
+₹ 7,704
+Total price: ₹ 44,682
 1 room × 5 nights incl. taxes &amp; fees
 Check Availability
 Sign in for member prices</t>
@@ -308,34 +329,10 @@
 Two-Bedroom Residence
 x4
 Free Cancellation
-₹ 18,844
-Total price: ₹ 117,772
-1 room × 5 nights incl. taxes &amp; fees
-Check Availability</t>
-  </si>
-  <si>
-    <t>Kester International Apartment Hotel
-Opened in 2025
-9.8/10
-Outstanding28 reviews
-"Great service"
-"Great rooms"
-Near Yaya CentreShow on Map
-Boutique 2-bedroom And 1-living Room Suite
-x4
-Entire apartment 95㎡
-2 bedrooms
-3 beds
-Earn ₹ 519.94 in Trip Coins
-Only 3 left at this price
-Special Discount
-15% off
-₹ 7,192
-₹ 5,970
-Total price: ₹ 34,623
-1 room × 5 nights incl. taxes &amp; fees
-Check Availability
-Sign in for member prices</t>
+₹ 18,849
+Total price: ₹ 117,805
+1 room × 5 nights incl. taxes &amp; fees
+Check Availability</t>
   </si>
   <si>
     <t>Lavington Residences By Trianum
@@ -377,7 +374,7 @@
 Entire apartment
 2 bedrooms
 2 beds
-Free Cancellation
+Member deal
 ₹ 6,945
 Total price: ₹ 40,941
 1 room × 5 nights incl. taxes &amp; fees
@@ -413,20 +410,6 @@
 ₹ 29,260
 Total price: ₹ 187,305
 1 room × 5 nights incl. taxes &amp; fees
-Check Availability</t>
-  </si>
-  <si>
-    <t>Mercure Nairobi Upper Hill
-Ad
-8.9/10
-Very good60 reviews
-Near Giraffe manorShow on Map
-2
-Classic Superior King Room
-Free Cancellation
-₹ 11,338
-Total price: ₹ 141,720
-2 rooms × 5 nights incl. taxes &amp; fees
 Check Availability</t>
   </si>
   <si>
@@ -439,9 +422,8 @@
 No. 3 of 4-Star Select Hotels in Nairobi
 2
 Deluxe Room With Two Double Beds
-Free Cancellation
 Earn ₹ 1,697.05 in Trip Coins
-Last booked 3 hrs ago
+Last booked 2 hrs ago
 ₹ 13,576
 Total price: ₹ 169,703
 2 rooms × 5 nights incl. taxes &amp; fees
@@ -553,24 +535,24 @@
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C6" t="s" s="0">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C7" t="s" s="0">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8">
@@ -578,15 +560,15 @@
         <v>11</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C8" t="s" s="0">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="B9" t="s" s="0">
         <v>20</v>
@@ -600,7 +582,7 @@
         <v>22</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="C10" t="s" s="0">
         <v>23</v>
@@ -608,10 +590,10 @@
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="C11" t="s" s="0">
         <v>24</v>
@@ -622,7 +604,7 @@
         <v>25</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13">

</xml_diff>